<commit_message>
50. Modificant full de calcul
</commit_message>
<xml_diff>
--- a/Fulldecàlcul.xlsx
+++ b/Fulldecàlcul.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>ESTIMACIÓ DEL TEMPS</t>
   </si>
@@ -163,15 +163,12 @@
     <t>Veure Newsletter</t>
   </si>
   <si>
+    <t>Visualitzar Ruta</t>
+  </si>
+  <si>
     <t>Mig</t>
   </si>
   <si>
-    <t>Visualitzar Ruta</t>
-  </si>
-  <si>
-    <t>Complex</t>
-  </si>
-  <si>
     <t>Consultar rutes temàtiques</t>
   </si>
   <si>
@@ -181,42 +178,9 @@
     <t>Visualitzar Botiga</t>
   </si>
   <si>
-    <t>Consultar ofertes i descomptes</t>
-  </si>
-  <si>
-    <t>Guardar botiga com a favorit</t>
-  </si>
-  <si>
-    <t>Compartir experiencia</t>
-  </si>
-  <si>
-    <t>Compartir Botiga</t>
-  </si>
-  <si>
     <t>Valorar Botiga</t>
   </si>
   <si>
-    <t>Donar Puntuació</t>
-  </si>
-  <si>
-    <t>Fer comentari</t>
-  </si>
-  <si>
-    <t>Compartir Valoració</t>
-  </si>
-  <si>
-    <t>Llistar Botigues per descompte</t>
-  </si>
-  <si>
-    <t>Llistar Botigues per tipus</t>
-  </si>
-  <si>
-    <t>Llistar Botigues per proximitat</t>
-  </si>
-  <si>
-    <t>Llistar Botigues favorites</t>
-  </si>
-  <si>
     <t>Demanar gestions del sisyema</t>
   </si>
   <si>
@@ -229,19 +193,43 @@
     <t>Eliminar Botiga</t>
   </si>
   <si>
-    <t>Afegir notícia</t>
-  </si>
-  <si>
-    <t>Afegir ruta temàtica</t>
-  </si>
-  <si>
-    <t>Editar ruta</t>
-  </si>
-  <si>
-    <t>Elimina Ruta</t>
+    <t>Gestionar  notícies</t>
+  </si>
+  <si>
+    <t>Gestionar  rutes temàtiques</t>
   </si>
   <si>
     <t>ESTIMACIÓ DEL PRESSUPOST</t>
+  </si>
+  <si>
+    <t>ESTIMACIÓ DEL TEMPS                    =</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UCP x PF</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Disciplina</t>
+  </si>
+  <si>
+    <t>Model d'empresa</t>
+  </si>
+  <si>
+    <t>Requeriments</t>
+  </si>
+  <si>
+    <t>Anàlisis i disseny</t>
+  </si>
+  <si>
+    <t>Implementació</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
   </si>
 </sst>
 </file>
@@ -380,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -488,6 +476,12 @@
     <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,7 +538,7 @@
       </c>
       <c r="E4" s="5" t="str">
         <f>(E6+E7)*E8*E9</f>
-        <v>20.80866667</v>
+        <v>46.0992</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -570,8 +564,8 @@
         <v>2</v>
       </c>
       <c r="E6" s="8" t="str">
-        <f>D78</f>
-        <v>8.666666667</v>
+        <f>D65</f>
+        <v>35</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="3"/>
@@ -1349,8 +1343,9 @@
       <c r="C52" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="27">
-        <v>5.0</v>
+      <c r="D52" s="27" t="str">
+        <f t="shared" ref="D52:D64" si="3">IF(C52 = "Simple", 5, IF(C52 = "Mig", 10, 15))</f>
+        <v>5</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -1363,11 +1358,12 @@
       <c r="B53" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="27">
-        <v>10.0</v>
+      <c r="C53" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -1378,13 +1374,14 @@
     <row r="54">
       <c r="A54" s="3"/>
       <c r="B54" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="27">
-        <v>15.0</v>
+      <c r="D54" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -1395,13 +1392,14 @@
     <row r="55">
       <c r="A55" s="3"/>
       <c r="B55" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="27">
-        <v>10.0</v>
+        <v>52</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -1412,13 +1410,14 @@
     <row r="56">
       <c r="A56" s="3"/>
       <c r="B56" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C56" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D56" s="27">
-        <v>5.0</v>
+      <c r="D56" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -1429,13 +1428,14 @@
     <row r="57">
       <c r="A57" s="3"/>
       <c r="B57" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D57" s="27">
-        <v>10.0</v>
+        <v>51</v>
+      </c>
+      <c r="D57" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -1446,13 +1446,14 @@
     <row r="58">
       <c r="A58" s="3"/>
       <c r="B58" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="27">
-        <v>15.0</v>
+        <v>48</v>
+      </c>
+      <c r="D58" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -1462,14 +1463,15 @@
     </row>
     <row r="59">
       <c r="A59" s="3"/>
-      <c r="B59" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="32" t="s">
+      <c r="B59" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D59" s="27">
-        <v>5.0</v>
+      <c r="D59" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -1479,14 +1481,15 @@
     </row>
     <row r="60">
       <c r="A60" s="3"/>
-      <c r="B60" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="32" t="s">
+      <c r="B60" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="27">
-        <v>5.0</v>
+      <c r="D60" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -1496,14 +1499,15 @@
     </row>
     <row r="61">
       <c r="A61" s="3"/>
-      <c r="B61" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C61" s="32" t="s">
+      <c r="B61" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="27">
-        <v>5.0</v>
+      <c r="D61" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -1513,14 +1517,15 @@
     </row>
     <row r="62">
       <c r="A62" s="3"/>
-      <c r="B62" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C62" s="32" t="s">
+      <c r="B62" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D62" s="27">
-        <v>5.0</v>
+      <c r="D62" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -1530,14 +1535,15 @@
     </row>
     <row r="63">
       <c r="A63" s="3"/>
-      <c r="B63" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C63" s="32" t="s">
+      <c r="B63" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D63" s="27">
-        <v>5.0</v>
+      <c r="D63" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -1547,14 +1553,15 @@
     </row>
     <row r="64">
       <c r="A64" s="3"/>
-      <c r="B64" s="14" t="s">
-        <v>62</v>
+      <c r="B64" s="27" t="s">
+        <v>61</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="27">
-        <v>5.0</v>
+        <v>51</v>
+      </c>
+      <c r="D64" s="27" t="str">
+        <f t="shared" si="3"/>
+        <v>10</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -1564,14 +1571,13 @@
     </row>
     <row r="65">
       <c r="A65" s="3"/>
-      <c r="B65" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="27">
-        <v>5.0</v>
+      <c r="B65" s="34"/>
+      <c r="C65" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="35" t="str">
+        <f>SUM(D59:D64)</f>
+        <v>35</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -1581,15 +1587,9 @@
     </row>
     <row r="66">
       <c r="A66" s="3"/>
-      <c r="B66" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D66" s="27">
-        <v>15.0</v>
-      </c>
+      <c r="B66" s="34"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -1598,15 +1598,9 @@
     </row>
     <row r="67">
       <c r="A67" s="3"/>
-      <c r="B67" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C67" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D67" s="27">
-        <v>15.0</v>
-      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -1614,236 +1608,76 @@
       <c r="I67" s="3"/>
     </row>
     <row r="68">
-      <c r="A68" s="3"/>
-      <c r="B68" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D68" s="27">
-        <v>15.0</v>
-      </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
+      <c r="A68" s="38"/>
+      <c r="B68" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
     </row>
     <row r="69">
       <c r="A69" s="3"/>
-      <c r="B69" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D69" s="27">
-        <v>10.0</v>
-      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
     </row>
-    <row r="70">
-      <c r="A70" s="3"/>
-      <c r="B70" s="27" t="s">
+    <row r="71" ht="21.0" customHeight="1">
+      <c r="B71" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C71" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" ht="21.0" customHeight="1">
+      <c r="C72" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" s="41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" s="41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D70" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-    </row>
-    <row r="71">
-      <c r="A71" s="3"/>
-      <c r="B71" s="27" t="s">
+    </row>
+    <row r="76">
+      <c r="B76" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D71" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="3"/>
-      <c r="B72" s="27" t="s">
+    </row>
+    <row r="77">
+      <c r="B77" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73">
-      <c r="A73" s="3"/>
-      <c r="B73" s="27" t="s">
+    </row>
+    <row r="78">
+      <c r="B78" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="27">
-        <v>5.0</v>
-      </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="3"/>
-      <c r="B74" s="27" t="s">
+    </row>
+    <row r="79">
+      <c r="B79" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="27">
-        <v>10.0</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="3"/>
-      <c r="B75" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="C75" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D75" s="27">
-        <v>10.0</v>
-      </c>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="3"/>
-      <c r="B76" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C76" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D76" s="27">
-        <v>10.0</v>
-      </c>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="3"/>
-      <c r="B77" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="27">
-        <v>10.0</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="3"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D78" s="35" t="str">
-        <f>AVERAGE(D63:D77)</f>
-        <v>8.666666667</v>
-      </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-    </row>
-    <row r="79">
-      <c r="A79" s="3"/>
-      <c r="B79" s="34"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-    </row>
-    <row r="80">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-    </row>
-    <row r="81">
-      <c r="A81" s="38"/>
-      <c r="B81" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="38"/>
-      <c r="H81" s="38"/>
-      <c r="I81" s="38"/>
-    </row>
-    <row r="82">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>